<commit_message>
added regions to excel file manually, due to format of data online
</commit_message>
<xml_diff>
--- a/ewp-conflicts-data.xlsx
+++ b/ewp-conflicts-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540"/>
+    <workbookView xWindow="1780" yWindow="460" windowWidth="28720" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="EVENT DATA" sheetId="1" r:id="rId1"/>
@@ -1151,7 +1151,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1173,6 +1173,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1228,7 +1234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1416,6 +1422,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1724,8 +1748,8 @@
   </sheetPr>
   <dimension ref="A1:L132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1799,7 +1823,7 @@
         <v>1956</v>
       </c>
       <c r="F2" s="8">
-        <f>E2-D2</f>
+        <f t="shared" ref="F2:F21" si="0">E2-D2</f>
         <v>12</v>
       </c>
       <c r="G2" s="9" t="s">
@@ -1812,7 +1836,7 @@
         <v>60138</v>
       </c>
       <c r="J2" s="52">
-        <f t="shared" ref="J2:J21" si="0">AVERAGE(H2:I2)</f>
+        <f t="shared" ref="J2:J21" si="1">AVERAGE(H2:I2)</f>
         <v>55138</v>
       </c>
       <c r="K2" s="22" t="s">
@@ -1839,7 +1863,7 @@
         <v>1985</v>
       </c>
       <c r="F3" s="8">
-        <f>E3-D3</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="G3" s="9" t="s">
@@ -1852,7 +1876,7 @@
         <v>10000</v>
       </c>
       <c r="J3" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7500</v>
       </c>
       <c r="K3" s="22" t="s">
@@ -1879,7 +1903,7 @@
         <v>1956</v>
       </c>
       <c r="F4" s="8">
-        <f>E4-D4</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -1892,7 +1916,7 @@
         <v>30000</v>
       </c>
       <c r="J4" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19334</v>
       </c>
       <c r="K4" s="22" t="s">
@@ -1919,7 +1943,7 @@
         <v>1960</v>
       </c>
       <c r="F5" s="8">
-        <f>E5-D5</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -1932,7 +1956,7 @@
         <v>2000</v>
       </c>
       <c r="J5" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="K5" s="22" t="s">
@@ -1943,7 +1967,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="265.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="57" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="45" t="s">
@@ -1959,7 +1983,7 @@
         <v>1989</v>
       </c>
       <c r="F6" s="8">
-        <f>E6-D6</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="G6" s="37" t="s">
@@ -1972,7 +1996,7 @@
         <v>360000</v>
       </c>
       <c r="J6" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>230000</v>
       </c>
       <c r="K6" s="44" t="s">
@@ -1999,7 +2023,7 @@
         <v>1948</v>
       </c>
       <c r="F7" s="8">
-        <f>E7-D7</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G7" s="39" t="s">
@@ -2012,7 +2036,7 @@
         <v>59355</v>
       </c>
       <c r="J7" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57177.5</v>
       </c>
       <c r="K7" s="23" t="s">
@@ -2023,7 +2047,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" s="11" customFormat="1" ht="354.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="58" t="s">
         <v>264</v>
       </c>
       <c r="B8" s="46" t="s">
@@ -2039,7 +2063,7 @@
         <v>1956</v>
       </c>
       <c r="F8" s="8">
-        <f>E8-D8</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -2052,7 +2076,7 @@
         <v>65000</v>
       </c>
       <c r="J8" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50000</v>
       </c>
       <c r="K8" s="22" t="s">
@@ -2079,7 +2103,7 @@
         <v>1946</v>
       </c>
       <c r="F9" s="8">
-        <f>E9-D9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G9" s="10" t="s">
@@ -2092,7 +2116,7 @@
         <v>30000</v>
       </c>
       <c r="J9" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24500</v>
       </c>
       <c r="K9" s="23" t="s">
@@ -2119,7 +2143,7 @@
         <v>1948</v>
       </c>
       <c r="F10" s="8">
-        <f>E10-D10</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G10" s="10" t="s">
@@ -2132,7 +2156,7 @@
         <v>1618400</v>
       </c>
       <c r="J10" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1421700</v>
       </c>
       <c r="K10" s="23" t="s">
@@ -2159,7 +2183,7 @@
         <v>1947</v>
       </c>
       <c r="F11" s="8">
-        <f>E11-D11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G11" s="10" t="s">
@@ -2172,7 +2196,7 @@
         <v>7500</v>
       </c>
       <c r="J11" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="K11" s="23" t="s">
@@ -2199,7 +2223,7 @@
         <v>1954</v>
       </c>
       <c r="F12" s="8">
-        <f>E12-D12</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -2212,7 +2236,7 @@
         <v>3000</v>
       </c>
       <c r="J12" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="K12" s="23" t="s">
@@ -2239,7 +2263,7 @@
         <v>1947</v>
       </c>
       <c r="F13" s="8">
-        <f>E13-D13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G13" s="10" t="s">
@@ -2252,7 +2276,7 @@
         <v>30000</v>
       </c>
       <c r="J13" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22500</v>
       </c>
       <c r="K13" s="23" t="s">
@@ -2279,7 +2303,7 @@
         <v>1963</v>
       </c>
       <c r="F14" s="8">
-        <f>E14-D14</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="G14" s="9" t="s">
@@ -2292,7 +2316,7 @@
         <v>25000</v>
       </c>
       <c r="J14" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18030</v>
       </c>
       <c r="K14" s="22" t="s">
@@ -2319,7 +2343,7 @@
         <v>1990</v>
       </c>
       <c r="F15" s="8">
-        <f>E15-D15</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="G15" s="6" t="s">
@@ -2332,7 +2356,7 @@
         <v>100000</v>
       </c>
       <c r="J15" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="K15" s="23" t="s">
@@ -2359,7 +2383,7 @@
         <v>1950</v>
       </c>
       <c r="F16" s="8">
-        <f>E16-D16</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G16" s="6" t="s">
@@ -2372,7 +2396,7 @@
         <v>30000</v>
       </c>
       <c r="J16" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21362.5</v>
       </c>
       <c r="K16" s="22" t="s">
@@ -2399,7 +2423,7 @@
         <v>1958</v>
       </c>
       <c r="F17" s="8">
-        <f>E17-D17</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G17" s="6" t="s">
@@ -2412,7 +2436,7 @@
         <v>150000</v>
       </c>
       <c r="J17" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="K17" s="23" t="s">
@@ -2439,7 +2463,7 @@
         <v>242</v>
       </c>
       <c r="F18" s="8" t="e">
-        <f>E18-D18</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -2452,7 +2476,7 @@
         <v>145000</v>
       </c>
       <c r="J18" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>145000</v>
       </c>
       <c r="K18" s="23" t="s">
@@ -2479,7 +2503,7 @@
         <v>242</v>
       </c>
       <c r="F19" s="8" t="e">
-        <f>E19-D19</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="G19" s="9" t="s">
@@ -2492,7 +2516,7 @@
         <v>1500000</v>
       </c>
       <c r="J19" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>950000</v>
       </c>
       <c r="K19" s="22" t="s">
@@ -2519,7 +2543,7 @@
         <v>1962</v>
       </c>
       <c r="F20" s="8">
-        <f>E20-D20</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="G20" s="6" t="s">
@@ -2532,7 +2556,7 @@
         <v>4000</v>
       </c>
       <c r="J20" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2750</v>
       </c>
       <c r="K20" s="22" t="s">
@@ -2559,7 +2583,7 @@
         <v>1977</v>
       </c>
       <c r="F21" s="8">
-        <f>E21-D21</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="G21" s="10" t="s">
@@ -2572,7 +2596,7 @@
         <v>40000000</v>
       </c>
       <c r="J21" s="52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35500000</v>
       </c>
       <c r="K21" s="22" t="s">
@@ -2621,7 +2645,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="39" x14ac:dyDescent="0.15">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="57" t="s">
         <v>287</v>
       </c>
       <c r="B23" s="45" t="s">
@@ -2637,7 +2661,7 @@
         <v>1975</v>
       </c>
       <c r="F23" s="8">
-        <f>E23-D23</f>
+        <f t="shared" ref="F23:F54" si="2">E23-D23</f>
         <v>21</v>
       </c>
       <c r="G23" s="37" t="s">
@@ -2650,7 +2674,7 @@
         <v>300000</v>
       </c>
       <c r="J23" s="52">
-        <f t="shared" ref="J23:J54" si="1">AVERAGE(H23:I23)</f>
+        <f t="shared" ref="J23:J54" si="3">AVERAGE(H23:I23)</f>
         <v>225000</v>
       </c>
       <c r="K23" s="22" t="s">
@@ -2661,7 +2685,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="189" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="59" t="s">
         <v>140</v>
       </c>
       <c r="B24" s="47"/>
@@ -2675,7 +2699,7 @@
         <v>1957</v>
       </c>
       <c r="F24" s="8">
-        <f>E24-D24</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="G24" s="39" t="s">
@@ -2688,7 +2712,7 @@
         <v>50000</v>
       </c>
       <c r="J24" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>41000</v>
       </c>
       <c r="K24" s="22" t="s">
@@ -2715,7 +2739,7 @@
         <v>1977</v>
       </c>
       <c r="F25" s="8">
-        <f>E25-D25</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="G25" s="9" t="s">
@@ -2728,7 +2752,7 @@
         <v>500000</v>
       </c>
       <c r="J25" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>375000</v>
       </c>
       <c r="K25" s="22" t="s">
@@ -2755,7 +2779,7 @@
         <v>1972</v>
       </c>
       <c r="F26" s="8">
-        <f>E26-D26</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G26" s="9" t="s">
@@ -2768,7 +2792,7 @@
         <v>600000</v>
       </c>
       <c r="J26" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>500000</v>
       </c>
       <c r="K26" s="22" t="s">
@@ -2795,7 +2819,7 @@
         <v>1986</v>
       </c>
       <c r="F27" s="8">
-        <f>E27-D27</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="G27" s="9" t="s">
@@ -2808,7 +2832,7 @@
         <v>60000</v>
       </c>
       <c r="J27" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>35000</v>
       </c>
       <c r="K27" s="22" t="s">
@@ -2835,7 +2859,7 @@
         <v>1970</v>
       </c>
       <c r="F28" s="8">
-        <f>E28-D28</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G28" s="6" t="s">
@@ -2848,7 +2872,7 @@
         <v>8335</v>
       </c>
       <c r="J28" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6667.5</v>
       </c>
       <c r="K28" s="22" t="s">
@@ -2875,7 +2899,7 @@
         <v>1959</v>
       </c>
       <c r="F29" s="8">
-        <f>E29-D29</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G29" s="6" t="s">
@@ -2888,7 +2912,7 @@
         <v>1000</v>
       </c>
       <c r="J29" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
       <c r="K29" s="22" t="s">
@@ -2899,7 +2923,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="164.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="59" t="s">
         <v>293</v>
       </c>
       <c r="B30" s="47" t="s">
@@ -2915,7 +2939,7 @@
         <v>1973</v>
       </c>
       <c r="F30" s="8">
-        <f>E30-D30</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G30" s="6" t="s">
@@ -2928,7 +2952,7 @@
         <v>90000</v>
       </c>
       <c r="J30" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>60000</v>
       </c>
       <c r="K30" s="23" t="s">
@@ -2939,7 +2963,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="204.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="57" t="s">
         <v>295</v>
       </c>
       <c r="B31" s="45" t="s">
@@ -2955,7 +2979,7 @@
         <v>1980</v>
       </c>
       <c r="F31" s="8">
-        <f>E31-D31</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="G31" s="37" t="s">
@@ -2968,7 +2992,7 @@
         <v>50000</v>
       </c>
       <c r="J31" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>28000</v>
       </c>
       <c r="K31" s="44" t="s">
@@ -2995,7 +3019,7 @@
         <v>1963</v>
       </c>
       <c r="F32" s="8">
-        <f>E32-D32</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="G32" s="6" t="s">
@@ -3008,7 +3032,7 @@
         <v>5000</v>
       </c>
       <c r="J32" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
       <c r="K32" s="23" t="s">
@@ -3035,7 +3059,7 @@
         <v>1991</v>
       </c>
       <c r="F33" s="8">
-        <f>E33-D33</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="G33" s="9" t="s">
@@ -3048,7 +3072,7 @@
         <v>240000</v>
       </c>
       <c r="J33" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>160000</v>
       </c>
       <c r="K33" s="22" t="s">
@@ -3075,7 +3099,7 @@
         <v>1991</v>
       </c>
       <c r="F34" s="8">
-        <f>E34-D34</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="G34" s="9" t="s">
@@ -3088,7 +3112,7 @@
         <v>200000</v>
       </c>
       <c r="J34" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>190000</v>
       </c>
       <c r="K34" s="22" t="s">
@@ -3115,7 +3139,7 @@
         <v>1962</v>
       </c>
       <c r="F35" s="8">
-        <f>E35-D35</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G35" s="9" t="s">
@@ -3128,7 +3152,7 @@
         <v>150000</v>
       </c>
       <c r="J35" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>90000</v>
       </c>
       <c r="K35" s="22" t="s">
@@ -3152,7 +3176,7 @@
         <v>1970</v>
       </c>
       <c r="F36" s="8">
-        <f>E36-D36</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G36" s="9" t="s">
@@ -3165,7 +3189,7 @@
         <v>50000</v>
       </c>
       <c r="J36" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>35000</v>
       </c>
       <c r="K36" s="22" t="s">
@@ -3192,7 +3216,7 @@
         <v>2003</v>
       </c>
       <c r="F37" s="8">
-        <f>E37-D37</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="G37" s="9" t="s">
@@ -3205,7 +3229,7 @@
         <v>85000</v>
       </c>
       <c r="J37" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>85000</v>
       </c>
       <c r="K37" s="22" t="s">
@@ -3230,7 +3254,7 @@
         <v>1967</v>
       </c>
       <c r="F38" s="8">
-        <f>E38-D38</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G38" s="9" t="s">
@@ -3243,7 +3267,7 @@
         <v>20000</v>
       </c>
       <c r="J38" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>16000</v>
       </c>
       <c r="K38" s="22" t="s">
@@ -3270,7 +3294,7 @@
         <v>1964</v>
       </c>
       <c r="F39" s="8">
-        <f>E39-D39</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G39" s="9" t="s">
@@ -3283,7 +3307,7 @@
         <v>5000</v>
       </c>
       <c r="J39" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4500</v>
       </c>
       <c r="K39" s="22" t="s">
@@ -3307,7 +3331,7 @@
         <v>1965</v>
       </c>
       <c r="F40" s="8">
-        <f>E40-D40</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G40" s="10" t="s">
@@ -3320,7 +3344,7 @@
         <v>5000</v>
       </c>
       <c r="J40" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3500</v>
       </c>
       <c r="K40" s="23" t="s">
@@ -3347,7 +3371,7 @@
         <v>1994</v>
       </c>
       <c r="F41" s="8">
-        <f>E41-D41</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="G41" s="10" t="s">
@@ -3360,7 +3384,7 @@
         <v>6000</v>
       </c>
       <c r="J41" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6000</v>
       </c>
       <c r="K41" s="23" t="s">
@@ -3385,7 +3409,7 @@
         <v>2010</v>
       </c>
       <c r="F42" s="8">
-        <f>E42-D42</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="G42" s="9" t="s">
@@ -3398,7 +3422,7 @@
         <v>60000</v>
       </c>
       <c r="J42" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>50000</v>
       </c>
       <c r="K42" s="22" t="s">
@@ -3425,7 +3449,7 @@
         <v>1978</v>
       </c>
       <c r="F43" s="8">
-        <f>E43-D43</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="G43" s="10" t="s">
@@ -3438,7 +3462,7 @@
         <v>5000</v>
       </c>
       <c r="J43" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4500</v>
       </c>
       <c r="K43" s="23" t="s">
@@ -3465,7 +3489,7 @@
         <v>1966</v>
       </c>
       <c r="F44" s="8">
-        <f>E44-D44</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G44" s="9" t="s">
@@ -3478,7 +3502,7 @@
         <v>500000</v>
       </c>
       <c r="J44" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>375000</v>
       </c>
       <c r="K44" s="22" t="s">
@@ -3503,7 +3527,7 @@
         <v>1973</v>
       </c>
       <c r="F45" s="8">
-        <f>E45-D45</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G45" s="9" t="s">
@@ -3516,7 +3540,7 @@
         <v>200000</v>
       </c>
       <c r="J45" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>150000</v>
       </c>
       <c r="K45" s="22" t="s">
@@ -3543,7 +3567,7 @@
         <v>1975</v>
       </c>
       <c r="F46" s="8">
-        <f>E46-D46</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G46" s="6" t="s">
@@ -3556,7 +3580,7 @@
         <v>200000</v>
       </c>
       <c r="J46" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>142500</v>
       </c>
       <c r="K46" s="18" t="s">
@@ -3583,7 +3607,7 @@
         <v>1970</v>
       </c>
       <c r="F47" s="8">
-        <f>E47-D47</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="G47" s="9" t="s">
@@ -3596,7 +3620,7 @@
         <v>2000000</v>
       </c>
       <c r="J47" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1300000</v>
       </c>
       <c r="K47" s="22" t="s">
@@ -3620,7 +3644,7 @@
         <v>1979</v>
       </c>
       <c r="F48" s="8">
-        <f>E48-D48</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G48" s="9" t="s">
@@ -3633,7 +3657,7 @@
         <v>50000</v>
       </c>
       <c r="J48" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45000</v>
       </c>
       <c r="K48" s="22" t="s">
@@ -3658,7 +3682,7 @@
         <v>2010</v>
       </c>
       <c r="F49" s="8">
-        <f>E49-D49</f>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="G49" s="30" t="s">
@@ -3671,7 +3695,7 @@
         <v>8000</v>
       </c>
       <c r="J49" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6500</v>
       </c>
       <c r="K49" s="31" t="s">
@@ -3696,7 +3720,7 @@
         <v>2007</v>
       </c>
       <c r="F50" s="8">
-        <f>E50-D50</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="G50" s="30" t="s">
@@ -3709,7 +3733,7 @@
         <v>40000</v>
       </c>
       <c r="J50" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>40000</v>
       </c>
       <c r="K50" s="31" t="s">
@@ -3733,7 +3757,7 @@
         <v>1971</v>
       </c>
       <c r="F51" s="8">
-        <f>E51-D51</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G51" s="9" t="s">
@@ -3746,7 +3770,7 @@
         <v>1000</v>
       </c>
       <c r="J51" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
       <c r="K51" s="22" t="s">
@@ -3770,7 +3794,7 @@
         <v>1979</v>
       </c>
       <c r="F52" s="8">
-        <f>E52-D52</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G52" s="9" t="s">
@@ -3783,7 +3807,7 @@
         <v>300000</v>
       </c>
       <c r="J52" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>165000</v>
       </c>
       <c r="K52" s="22" t="s">
@@ -3807,7 +3831,7 @@
         <v>1971</v>
       </c>
       <c r="F53" s="8">
-        <f>E53-D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G53" s="9" t="s">
@@ -3820,7 +3844,7 @@
         <v>1000000</v>
       </c>
       <c r="J53" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>650000</v>
       </c>
       <c r="K53" s="22" t="s">
@@ -3844,7 +3868,7 @@
         <v>1971</v>
       </c>
       <c r="F54" s="8">
-        <f>E54-D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G54" s="9" t="s">
@@ -3857,7 +3881,7 @@
         <v>8000</v>
       </c>
       <c r="J54" s="52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
       <c r="K54" s="22" t="s">
@@ -3881,7 +3905,7 @@
         <v>1986</v>
       </c>
       <c r="F55" s="8">
-        <f>E55-D55</f>
+        <f t="shared" ref="F55:F86" si="4">E55-D55</f>
         <v>14</v>
       </c>
       <c r="G55" s="9" t="s">
@@ -3894,7 +3918,7 @@
         <v>60000</v>
       </c>
       <c r="J55" s="52">
-        <f t="shared" ref="J55:J86" si="2">AVERAGE(H55:I55)</f>
+        <f t="shared" ref="J55:J86" si="5">AVERAGE(H55:I55)</f>
         <v>45000</v>
       </c>
       <c r="K55" s="22" t="s">
@@ -3921,7 +3945,7 @@
         <v>1979</v>
       </c>
       <c r="F56" s="8">
-        <f>E56-D56</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G56" s="9" t="s">
@@ -3934,7 +3958,7 @@
         <v>10000</v>
       </c>
       <c r="J56" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7000</v>
       </c>
       <c r="K56" s="22" t="s">
@@ -3959,7 +3983,7 @@
         <v>1977</v>
       </c>
       <c r="F57" s="8">
-        <f>E57-D57</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="G57" s="9" t="s">
@@ -3972,7 +3996,7 @@
         <v>2500</v>
       </c>
       <c r="J57" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1750</v>
       </c>
       <c r="K57" s="22" t="s">
@@ -3996,7 +4020,7 @@
         <v>1978</v>
       </c>
       <c r="F58" s="8">
-        <f>E58-D58</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="G58" s="9" t="s">
@@ -4009,7 +4033,7 @@
         <v>3200</v>
       </c>
       <c r="J58" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3200</v>
       </c>
       <c r="K58" s="22" t="s">
@@ -4036,7 +4060,7 @@
         <v>1991</v>
       </c>
       <c r="F59" s="8">
-        <f>E59-D59</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G59" s="9" t="s">
@@ -4049,7 +4073,7 @@
         <v>300000</v>
       </c>
       <c r="J59" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>250000</v>
       </c>
       <c r="K59" s="22" t="s">
@@ -4073,7 +4097,7 @@
         <v>1979</v>
       </c>
       <c r="F60" s="8">
-        <f>E60-D60</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="G60" s="9" t="s">
@@ -4086,7 +4110,7 @@
         <v>7000</v>
       </c>
       <c r="J60" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7000</v>
       </c>
       <c r="K60" s="22" t="s">
@@ -4113,7 +4137,7 @@
         <v>1991</v>
       </c>
       <c r="F61" s="8">
-        <f>E61-D61</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="G61" s="10" t="s">
@@ -4126,7 +4150,7 @@
         <v>36000</v>
       </c>
       <c r="J61" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>20500</v>
       </c>
       <c r="K61" s="23" t="s">
@@ -4150,7 +4174,7 @@
         <v>1979</v>
       </c>
       <c r="F62" s="8">
-        <f>E62-D62</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
@@ -4163,7 +4187,7 @@
         <v>2000000</v>
       </c>
       <c r="J62" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1500000</v>
       </c>
       <c r="K62" s="23" t="s">
@@ -4190,7 +4214,7 @@
         <v>1986</v>
       </c>
       <c r="F63" s="8">
-        <f>E63-D63</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G63" s="9" t="s">
@@ -4203,7 +4227,7 @@
         <v>100000</v>
       </c>
       <c r="J63" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>82500</v>
       </c>
       <c r="K63" s="22" t="s">
@@ -4227,7 +4251,7 @@
         <v>1992</v>
       </c>
       <c r="F64" s="8">
-        <f>E64-D64</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G64" s="9" t="s">
@@ -4240,7 +4264,7 @@
         <v>60000</v>
       </c>
       <c r="J64" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>31500</v>
       </c>
       <c r="K64" s="22" t="s">
@@ -4267,7 +4291,7 @@
         <v>2002</v>
       </c>
       <c r="F65" s="8">
-        <f>E65-D65</f>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="G65" s="9" t="s">
@@ -4280,7 +4304,7 @@
         <v>375000</v>
       </c>
       <c r="J65" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>217500</v>
       </c>
       <c r="K65" s="22" t="s">
@@ -4304,7 +4328,7 @@
         <v>1999</v>
       </c>
       <c r="F66" s="8">
-        <f>E66-D66</f>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="G66" s="9" t="s">
@@ -4317,7 +4341,7 @@
         <v>150000</v>
       </c>
       <c r="J66" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>115000</v>
       </c>
       <c r="K66" s="22" t="s">
@@ -4341,7 +4365,7 @@
         <v>1983</v>
       </c>
       <c r="F67" s="8">
-        <f>E67-D67</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G67" s="9" t="s">
@@ -4354,7 +4378,7 @@
         <v>30000</v>
       </c>
       <c r="J67" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>19500</v>
       </c>
       <c r="K67" s="22" t="s">
@@ -4379,7 +4403,7 @@
         <v>1994</v>
       </c>
       <c r="F68" s="8">
-        <f>E68-D68</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G68" s="12" t="s">
@@ -4392,7 +4416,7 @@
         <v>2700</v>
       </c>
       <c r="J68" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2700</v>
       </c>
       <c r="K68" s="22" t="s">
@@ -4416,7 +4440,7 @@
         <v>1985</v>
       </c>
       <c r="F69" s="8">
-        <f>E69-D69</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G69" s="9" t="s">
@@ -4429,7 +4453,7 @@
         <v>60000</v>
       </c>
       <c r="J69" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>50000</v>
       </c>
       <c r="K69" s="22" t="s">
@@ -4454,7 +4478,7 @@
         <v>1992</v>
       </c>
       <c r="F70" s="8">
-        <f>E70-D70</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="G70" s="10" t="s">
@@ -4467,7 +4491,7 @@
         <v>70000</v>
       </c>
       <c r="J70" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>55000</v>
       </c>
       <c r="K70" s="23" t="s">
@@ -4494,7 +4518,7 @@
         <v>1979</v>
       </c>
       <c r="F71" s="8">
-        <f>E71-D71</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G71" s="9" t="s">
@@ -4507,7 +4531,7 @@
         <v>3000</v>
       </c>
       <c r="J71" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2500</v>
       </c>
       <c r="K71" s="22" t="s">
@@ -4531,7 +4555,7 @@
         <v>1992</v>
       </c>
       <c r="F72" s="8">
-        <f>E72-D72</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G72" s="9" t="s">
@@ -4544,7 +4568,7 @@
         <v>1800000</v>
       </c>
       <c r="J72" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1400000</v>
       </c>
       <c r="K72" s="22" t="s">
@@ -4571,7 +4595,7 @@
         <v>2010</v>
       </c>
       <c r="F73" s="8">
-        <f>E73-D73</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="G73" s="9" t="s">
@@ -4584,7 +4608,7 @@
         <v>20000</v>
       </c>
       <c r="J73" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>15000</v>
       </c>
       <c r="K73" s="22" t="s">
@@ -4608,7 +4632,7 @@
         <v>1985</v>
       </c>
       <c r="F74" s="8">
-        <f>E74-D74</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="G74" s="12" t="s">
@@ -4621,7 +4645,7 @@
         <v>25000</v>
       </c>
       <c r="J74" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>17500</v>
       </c>
       <c r="K74" s="22" t="s">
@@ -4648,7 +4672,7 @@
         <v>1997</v>
       </c>
       <c r="F75" s="8">
-        <f>E75-D75</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G75" s="9" t="s">
@@ -4661,7 +4685,7 @@
         <v>2500</v>
       </c>
       <c r="J75" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2250</v>
       </c>
       <c r="K75" s="22" t="s">
@@ -4672,7 +4696,7 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="307.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="20" t="s">
+      <c r="A76" s="60" t="s">
         <v>320</v>
       </c>
       <c r="C76" s="8">
@@ -4685,7 +4709,7 @@
         <v>1992</v>
       </c>
       <c r="F76" s="8">
-        <f>E76-D76</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G76" s="12" t="s">
@@ -4698,7 +4722,7 @@
         <v>25000</v>
       </c>
       <c r="J76" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>25000</v>
       </c>
       <c r="K76" s="22" t="s">
@@ -4709,7 +4733,7 @@
       </c>
     </row>
     <row r="77" spans="1:12" ht="246.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="20" t="s">
+      <c r="A77" s="60" t="s">
         <v>308</v>
       </c>
       <c r="C77" s="8">
@@ -4722,7 +4746,7 @@
         <v>1980</v>
       </c>
       <c r="F77" s="8">
-        <f>E77-D77</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G77" s="37" t="s">
@@ -4735,7 +4759,7 @@
         <v>4200</v>
       </c>
       <c r="J77" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4100</v>
       </c>
       <c r="K77" s="22" t="s">
@@ -4762,7 +4786,7 @@
         <v>1986</v>
       </c>
       <c r="F78" s="8">
-        <f>E78-D78</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="G78" s="9" t="s">
@@ -4775,7 +4799,7 @@
         <v>300000</v>
       </c>
       <c r="J78" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>250000</v>
       </c>
       <c r="K78" s="22" t="s">
@@ -4799,7 +4823,7 @@
         <v>1988</v>
       </c>
       <c r="F79" s="8">
-        <f>E79-D79</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G79" s="12" t="s">
@@ -4812,7 +4836,7 @@
         <v>2000</v>
       </c>
       <c r="J79" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1500</v>
       </c>
       <c r="K79" s="22" t="s">
@@ -4836,7 +4860,7 @@
         <v>1987</v>
       </c>
       <c r="F80" s="8">
-        <f>E80-D80</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="G80" s="12" t="s">
@@ -4849,7 +4873,7 @@
         <v>20000</v>
       </c>
       <c r="J80" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>20000</v>
       </c>
       <c r="K80" s="22" t="s">
@@ -4873,7 +4897,7 @@
         <v>1990</v>
       </c>
       <c r="F81" s="8">
-        <f>E81-D81</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G81" s="9" t="s">
@@ -4886,7 +4910,7 @@
         <v>55000</v>
       </c>
       <c r="J81" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>55000</v>
       </c>
       <c r="K81" s="22" t="s">
@@ -4910,7 +4934,7 @@
         <v>1990</v>
       </c>
       <c r="F82" s="8">
-        <f>E82-D82</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G82" s="9" t="s">
@@ -4923,7 +4947,7 @@
         <v>40000</v>
       </c>
       <c r="J82" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>26000</v>
       </c>
       <c r="K82" s="22" t="s">
@@ -4947,7 +4971,7 @@
         <v>2005</v>
       </c>
       <c r="F83" s="8">
-        <f>E83-D83</f>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="G83" s="9" t="s">
@@ -4960,7 +4984,7 @@
         <v>2000000</v>
       </c>
       <c r="J83" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1750000</v>
       </c>
       <c r="K83" s="22" t="s">
@@ -4985,7 +5009,7 @@
         <v>2002</v>
       </c>
       <c r="F84" s="8">
-        <f>E84-D84</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="G84" s="12" t="s">
@@ -4998,7 +5022,7 @@
         <v>20000</v>
       </c>
       <c r="J84" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>16000</v>
       </c>
       <c r="K84" s="22" t="s">
@@ -5023,7 +5047,7 @@
         <v>1994</v>
       </c>
       <c r="F85" s="8">
-        <f>E85-D85</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G85" s="9" t="s">
@@ -5036,7 +5060,7 @@
         <v>3000</v>
       </c>
       <c r="J85" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3000</v>
       </c>
       <c r="K85" s="22" t="s">
@@ -5061,7 +5085,7 @@
         <v>1999</v>
       </c>
       <c r="F86" s="8">
-        <f>E86-D86</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="G86" s="9" t="s">
@@ -5074,7 +5098,7 @@
         <v>17500</v>
       </c>
       <c r="J86" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>17500</v>
       </c>
       <c r="K86" s="22" t="s">
@@ -5099,7 +5123,7 @@
         <v>1986</v>
       </c>
       <c r="F87" s="8">
-        <f>E87-D87</f>
+        <f t="shared" ref="F87:F118" si="6">E87-D87</f>
         <v>0</v>
       </c>
       <c r="G87" s="10" t="s">
@@ -5112,7 +5136,7 @@
         <v>2000</v>
       </c>
       <c r="J87" s="52">
-        <f t="shared" ref="J87:J118" si="3">AVERAGE(H87:I87)</f>
+        <f t="shared" ref="J87:J118" si="7">AVERAGE(H87:I87)</f>
         <v>1500</v>
       </c>
       <c r="K87" s="23" t="s">
@@ -5137,7 +5161,7 @@
         <v>2006</v>
       </c>
       <c r="F88" s="8">
-        <f>E88-D88</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="G88" s="10" t="s">
@@ -5150,7 +5174,7 @@
         <v>2000</v>
       </c>
       <c r="J88" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1500</v>
       </c>
       <c r="K88" s="23" t="s">
@@ -5177,7 +5201,7 @@
         <v>1988</v>
       </c>
       <c r="F89" s="8">
-        <f>E89-D89</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G89" s="10" t="s">
@@ -5190,7 +5214,7 @@
         <v>3000</v>
       </c>
       <c r="J89" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3000</v>
       </c>
       <c r="K89" s="23" t="s">
@@ -5215,7 +5239,7 @@
         <v>2005</v>
       </c>
       <c r="F90" s="40">
-        <f>E90-D90</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="G90" s="39" t="s">
@@ -5228,7 +5252,7 @@
         <v>200000</v>
       </c>
       <c r="J90" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>175000</v>
       </c>
       <c r="K90" s="23" t="s">
@@ -5239,7 +5263,7 @@
       </c>
     </row>
     <row r="91" spans="1:12" ht="286.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="20" t="s">
+      <c r="A91" s="60" t="s">
         <v>234</v>
       </c>
       <c r="C91" s="38">
@@ -5252,7 +5276,7 @@
         <v>1992</v>
       </c>
       <c r="F91" s="8">
-        <f>E91-D91</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G91" s="37" t="s">
@@ -5265,7 +5289,7 @@
         <v>60000</v>
       </c>
       <c r="J91" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>42500</v>
       </c>
       <c r="K91" s="44" t="s">
@@ -5276,7 +5300,7 @@
       </c>
     </row>
     <row r="92" spans="1:12" ht="115.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="16" t="s">
+      <c r="A92" s="57" t="s">
         <v>326</v>
       </c>
       <c r="C92" s="40">
@@ -5289,7 +5313,7 @@
         <v>1998</v>
       </c>
       <c r="F92" s="8">
-        <f>E92-D92</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="G92" s="39" t="s">
@@ -5302,7 +5326,7 @@
         <v>15000</v>
       </c>
       <c r="J92" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>11250</v>
       </c>
       <c r="K92" s="23" t="s">
@@ -5313,7 +5337,7 @@
       </c>
     </row>
     <row r="93" spans="1:12" ht="183.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="19" t="s">
+      <c r="A93" s="61" t="s">
         <v>280</v>
       </c>
       <c r="B93" s="47"/>
@@ -5327,7 +5351,7 @@
         <v>2005</v>
       </c>
       <c r="F93" s="8">
-        <f>E93-D93</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="G93" s="9" t="s">
@@ -5340,7 +5364,7 @@
         <v>11000</v>
       </c>
       <c r="J93" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9000</v>
       </c>
       <c r="K93" s="22" t="s">
@@ -5365,7 +5389,7 @@
         <v>1989</v>
       </c>
       <c r="F94" s="8">
-        <f>E94-D94</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G94" s="9" t="s">
@@ -5378,7 +5402,7 @@
         <v>1000</v>
       </c>
       <c r="J94" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
       <c r="K94" s="22" t="s">
@@ -5405,7 +5429,7 @@
         <v>1990</v>
       </c>
       <c r="F95" s="8">
-        <f>E95-D95</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G95" s="9" t="s">
@@ -5418,7 +5442,7 @@
         <v>15000</v>
       </c>
       <c r="J95" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>11250</v>
       </c>
       <c r="K95" s="22" t="s">
@@ -5442,7 +5466,7 @@
         <v>2011</v>
       </c>
       <c r="F96" s="8">
-        <f>E96-D96</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="G96" s="9" t="s">
@@ -5455,7 +5479,7 @@
         <v>30000</v>
       </c>
       <c r="J96" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>30000</v>
       </c>
       <c r="K96" s="22" t="s">
@@ -5479,7 +5503,7 @@
         <v>1994</v>
       </c>
       <c r="F97" s="8">
-        <f>E97-D97</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G97" s="9" t="s">
@@ -5492,7 +5516,7 @@
         <v>800000</v>
       </c>
       <c r="J97" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>650000</v>
       </c>
       <c r="K97" s="22" t="s">
@@ -5516,7 +5540,7 @@
         <v>2009</v>
       </c>
       <c r="F98" s="8">
-        <f>E98-D98</f>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="G98" s="9" t="s">
@@ -5529,7 +5553,7 @@
         <v>4500</v>
       </c>
       <c r="J98" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4500</v>
       </c>
       <c r="K98" s="22" t="s">
@@ -5553,7 +5577,7 @@
         <v>2003</v>
       </c>
       <c r="F99" s="8">
-        <f>E99-D99</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="G99" s="9" t="s">
@@ -5566,7 +5590,7 @@
         <v>60000</v>
       </c>
       <c r="J99" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>45000</v>
       </c>
       <c r="K99" s="22" t="s">
@@ -5590,7 +5614,7 @@
         <v>2002</v>
       </c>
       <c r="F100" s="8">
-        <f>E100-D100</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="G100" s="9" t="s">
@@ -5603,7 +5627,7 @@
         <v>7000</v>
       </c>
       <c r="J100" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4500</v>
       </c>
       <c r="K100" s="22" t="s">
@@ -5627,7 +5651,7 @@
         <v>2005</v>
       </c>
       <c r="F101" s="8">
-        <f>E101-D101</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="G101" s="9" t="s">
@@ -5640,7 +5664,7 @@
         <v>50000</v>
       </c>
       <c r="J101" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>37500</v>
       </c>
       <c r="K101" s="22" t="s">
@@ -5667,7 +5691,7 @@
         <v>1992</v>
       </c>
       <c r="F102" s="8">
-        <f>E102-D102</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G102" s="9" t="s">
@@ -5680,7 +5704,7 @@
         <v>4000</v>
       </c>
       <c r="J102" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3500</v>
       </c>
       <c r="K102" s="22" t="s">
@@ -5704,7 +5728,7 @@
         <v>1994</v>
       </c>
       <c r="F103" s="8">
-        <f>E103-D103</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="G103" s="9" t="s">
@@ -5717,7 +5741,7 @@
         <v>1500</v>
       </c>
       <c r="J103" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1500</v>
       </c>
       <c r="K103" s="22" t="s">
@@ -5744,7 +5768,7 @@
         <v>1994</v>
       </c>
       <c r="F104" s="8">
-        <f>E104-D104</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="G104" s="9" t="s">
@@ -5757,7 +5781,7 @@
         <v>4000</v>
       </c>
       <c r="J104" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3500</v>
       </c>
       <c r="K104" s="22" t="s">
@@ -5784,7 +5808,7 @@
         <v>2003</v>
       </c>
       <c r="F105" s="8">
-        <f>E105-D105</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="G105" s="9" t="s">
@@ -5797,7 +5821,7 @@
         <v>2000</v>
       </c>
       <c r="J105" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1500</v>
       </c>
       <c r="K105" s="22" t="s">
@@ -5821,7 +5845,7 @@
         <v>1995</v>
       </c>
       <c r="F106" s="8">
-        <f>E106-D106</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="G106" s="9" t="s">
@@ -5834,7 +5858,7 @@
         <v>145000</v>
       </c>
       <c r="J106" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>145000</v>
       </c>
       <c r="K106" s="22" t="s">
@@ -5858,7 +5882,7 @@
         <v>1996</v>
       </c>
       <c r="F107" s="8">
-        <f>E107-D107</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G107" s="9" t="s">
@@ -5871,7 +5895,7 @@
         <v>10000</v>
       </c>
       <c r="J107" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>6250</v>
       </c>
       <c r="K107" s="22" t="s">
@@ -5895,7 +5919,7 @@
         <v>1997</v>
       </c>
       <c r="F108" s="8">
-        <f>E108-D108</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="G108" s="9" t="s">
@@ -5908,7 +5932,7 @@
         <v>25000</v>
       </c>
       <c r="J108" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>17500</v>
       </c>
       <c r="K108" s="22" t="s">
@@ -5932,7 +5956,7 @@
         <v>1993</v>
       </c>
       <c r="F109" s="8">
-        <f>E109-D109</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G109" s="9" t="s">
@@ -5945,7 +5969,7 @@
         <v>2000</v>
       </c>
       <c r="J109" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2000</v>
       </c>
       <c r="K109" s="22" t="s">
@@ -5969,7 +5993,7 @@
         <v>1997</v>
       </c>
       <c r="F110" s="8">
-        <f>E110-D110</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G110" s="37" t="s">
@@ -5982,7 +6006,7 @@
         <v>10000</v>
       </c>
       <c r="J110" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9000</v>
       </c>
       <c r="K110" s="44" t="s">
@@ -6006,7 +6030,7 @@
         <v>1997</v>
       </c>
       <c r="F111" s="8">
-        <f>E111-D111</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G111" s="39" t="s">
@@ -6019,7 +6043,7 @@
         <v>5000</v>
       </c>
       <c r="J111" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>5000</v>
       </c>
       <c r="K111" s="23" t="s">
@@ -6043,7 +6067,7 @@
         <v>1999</v>
       </c>
       <c r="F112" s="8">
-        <f>E112-D112</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="G112" s="9" t="s">
@@ -6056,7 +6080,7 @@
         <v>13000</v>
       </c>
       <c r="J112" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>13000</v>
       </c>
       <c r="K112" s="22" t="s">
@@ -6080,7 +6104,7 @@
         <v>2009</v>
       </c>
       <c r="F113" s="8">
-        <f>E113-D113</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="G113" s="9" t="s">
@@ -6093,7 +6117,7 @@
         <v>70000</v>
       </c>
       <c r="J113" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>62500</v>
       </c>
       <c r="K113" s="22" t="s">
@@ -6118,7 +6142,7 @@
         <v>2006</v>
       </c>
       <c r="F114" s="8">
-        <f>E114-D114</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="G114" s="9" t="s">
@@ -6131,7 +6155,7 @@
         <v>7000</v>
       </c>
       <c r="J114" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7000</v>
       </c>
       <c r="K114" s="22" t="s">
@@ -6156,7 +6180,7 @@
         <v>2001</v>
       </c>
       <c r="F115" s="8">
-        <f>E115-D115</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="G115" s="9" t="s">
@@ -6169,7 +6193,7 @@
         <v>10000</v>
       </c>
       <c r="J115" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7500</v>
       </c>
       <c r="K115" s="22" t="s">
@@ -6193,7 +6217,7 @@
         <v>2003</v>
       </c>
       <c r="F116" s="8">
-        <f>E116-D116</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="G116" s="10" t="s">
@@ -6206,7 +6230,7 @@
         <v>5000</v>
       </c>
       <c r="J116" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4000</v>
       </c>
       <c r="K116" s="23" t="s">
@@ -6230,7 +6254,7 @@
         <v>1999</v>
       </c>
       <c r="F117" s="8">
-        <f>E117-D117</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G117" s="9" t="s">
@@ -6243,7 +6267,7 @@
         <v>10000</v>
       </c>
       <c r="J117" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>10000</v>
       </c>
       <c r="K117" s="22" t="s">
@@ -6267,7 +6291,7 @@
         <v>242</v>
       </c>
       <c r="F118" s="8" t="e">
-        <f>E118-D118</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="G118" s="9" t="s">
@@ -6280,7 +6304,7 @@
         <v>100000</v>
       </c>
       <c r="J118" s="52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>100000</v>
       </c>
       <c r="K118" s="22" t="s">
@@ -6304,7 +6328,7 @@
         <v>2003</v>
       </c>
       <c r="F119" s="8">
-        <f>E119-D119</f>
+        <f t="shared" ref="F119:F150" si="8">E119-D119</f>
         <v>4</v>
       </c>
       <c r="G119" s="9" t="s">
@@ -6317,7 +6341,7 @@
         <v>1000</v>
       </c>
       <c r="J119" s="52">
-        <f t="shared" ref="J119:J129" si="4">AVERAGE(H119:I119)</f>
+        <f t="shared" ref="J119:J129" si="9">AVERAGE(H119:I119)</f>
         <v>1000</v>
       </c>
       <c r="K119" s="22" t="s">
@@ -6341,7 +6365,7 @@
         <v>242</v>
       </c>
       <c r="F120" s="8" t="e">
-        <f>E120-D120</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G120" s="9" t="s">
@@ -6354,7 +6378,7 @@
         <v>300000</v>
       </c>
       <c r="J120" s="52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>250000</v>
       </c>
       <c r="K120" s="22" t="s">
@@ -6378,7 +6402,7 @@
         <v>2009</v>
       </c>
       <c r="F121" s="8">
-        <f>E121-D121</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G121" s="9" t="s">
@@ -6391,7 +6415,7 @@
         <v>20000</v>
       </c>
       <c r="J121" s="52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>11500</v>
       </c>
       <c r="K121" s="22" t="s">
@@ -6416,7 +6440,7 @@
         <v>242</v>
       </c>
       <c r="F122" s="38" t="e">
-        <f>E122-D122</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G122" s="37" t="s">
@@ -6429,7 +6453,7 @@
         <v>3000</v>
       </c>
       <c r="J122" s="52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>2000</v>
       </c>
       <c r="K122" s="44" t="s">
@@ -6451,7 +6475,7 @@
         <v>2011</v>
       </c>
       <c r="F123" s="8">
-        <f>E123-D123</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G123" s="9" t="s">
@@ -6464,7 +6488,7 @@
         <v>3000</v>
       </c>
       <c r="J123" s="52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>2250</v>
       </c>
       <c r="K123" s="22" t="s">
@@ -6488,7 +6512,7 @@
         <v>2011</v>
       </c>
       <c r="F124" s="8">
-        <f>E124-D124</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G124" s="9" t="s">
@@ -6501,7 +6525,7 @@
         <v>2000</v>
       </c>
       <c r="J124" s="52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1300</v>
       </c>
       <c r="K124" s="22" t="s">
@@ -6525,7 +6549,7 @@
         <v>242</v>
       </c>
       <c r="F125" s="8" t="e">
-        <f>E125-D125</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G125" s="9" t="s">
@@ -6538,7 +6562,7 @@
         <v>48000</v>
       </c>
       <c r="J125" s="52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>35250</v>
       </c>
       <c r="K125" s="22" t="s">
@@ -6563,7 +6587,7 @@
         <v>242</v>
       </c>
       <c r="F126" s="8" t="e">
-        <f>E126-D126</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G126" s="9" t="s">
@@ -6576,7 +6600,7 @@
         <v>2000</v>
       </c>
       <c r="J126" s="52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1500</v>
       </c>
       <c r="K126" s="22" t="s">
@@ -6601,7 +6625,7 @@
         <v>242</v>
       </c>
       <c r="F127" s="38" t="e">
-        <f>E127-D127</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G127" s="37" t="s">
@@ -6614,7 +6638,7 @@
         <v>1400</v>
       </c>
       <c r="J127" s="52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1200</v>
       </c>
       <c r="K127" s="44"/>
@@ -6634,7 +6658,7 @@
         <v>242</v>
       </c>
       <c r="F128" s="8" t="e">
-        <f>E128-D128</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G128" s="9" t="s">
@@ -6647,7 +6671,7 @@
         <v>37500</v>
       </c>
       <c r="J128" s="52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>23750</v>
       </c>
       <c r="K128" s="22" t="s">
@@ -6672,7 +6696,7 @@
         <v>242</v>
       </c>
       <c r="F129" s="38" t="e">
-        <f>E129-D129</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G129" s="37" t="s">
@@ -6685,7 +6709,7 @@
         <v>3000</v>
       </c>
       <c r="J129" s="52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>2000</v>
       </c>
       <c r="K129" s="44" t="s">

</xml_diff>